<commit_message>
r u read these
</commit_message>
<xml_diff>
--- a/LR3/table_1_30.xlsx
+++ b/LR3/table_1_30.xlsx
@@ -3,14 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157FCDBD-7065-460A-AC28-094B139A2D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E29AE89-9AF7-436B-96A4-8CBC6795B6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -200,7 +198,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -223,17 +220,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -576,9 +570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -599,74 +591,74 @@
       </c>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="3"/>
-      <c r="AH2" s="3"/>
-      <c r="AI2" s="3"/>
-      <c r="AJ2" s="3"/>
-      <c r="AK2" s="3"/>
-      <c r="AL2" s="3"/>
-      <c r="AM2" s="3"/>
-      <c r="AN2" s="3"/>
-      <c r="AO2" s="3"/>
-      <c r="AP2" s="3"/>
-      <c r="AQ2" s="3"/>
+      <c r="K2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -683,10 +675,10 @@
         <f>D3*C3</f>
         <v>1617</v>
       </c>
-      <c r="F3" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G3" s="5">
+      <c r="F3" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G3" s="4">
         <v>44805</v>
       </c>
       <c r="H3" s="1">
@@ -705,7 +697,7 @@
       </c>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -722,10 +714,10 @@
         <f t="shared" ref="E4:E38" si="0">D4*C4</f>
         <v>1681.9</v>
       </c>
-      <c r="F4" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G4" s="5">
+      <c r="F4" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G4" s="4">
         <v>44806</v>
       </c>
       <c r="H4" s="1">
@@ -744,7 +736,7 @@
       </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -761,10 +753,10 @@
         <f t="shared" si="0"/>
         <v>1745.7</v>
       </c>
-      <c r="F5" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G5" s="5">
+      <c r="F5" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G5" s="4">
         <v>44807</v>
       </c>
       <c r="H5" s="1">
@@ -783,7 +775,7 @@
       </c>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -800,10 +792,10 @@
         <f t="shared" si="0"/>
         <v>1808.4</v>
       </c>
-      <c r="F6" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G6" s="5">
+      <c r="F6" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G6" s="4">
         <v>44808</v>
       </c>
       <c r="H6" s="1">
@@ -822,7 +814,7 @@
       </c>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -839,10 +831,10 @@
         <f t="shared" si="0"/>
         <v>1870.0000000000002</v>
       </c>
-      <c r="F7" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G7" s="5">
+      <c r="F7" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G7" s="4">
         <v>44809</v>
       </c>
       <c r="H7" s="1">
@@ -861,7 +853,7 @@
       </c>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -878,10 +870,10 @@
         <f t="shared" si="0"/>
         <v>1930.5</v>
       </c>
-      <c r="F8" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G8" s="5">
+      <c r="F8" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G8" s="4">
         <v>44810</v>
       </c>
       <c r="H8" s="1">
@@ -900,7 +892,7 @@
       </c>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -917,10 +909,10 @@
         <f t="shared" si="0"/>
         <v>1989.9</v>
       </c>
-      <c r="F9" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G9" s="5">
+      <c r="F9" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G9" s="4">
         <v>44811</v>
       </c>
       <c r="H9" s="1">
@@ -939,7 +931,7 @@
       </c>
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -956,10 +948,10 @@
         <f t="shared" si="0"/>
         <v>2048.2000000000003</v>
       </c>
-      <c r="F10" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G10" s="5">
+      <c r="F10" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G10" s="4">
         <v>44812</v>
       </c>
       <c r="H10" s="1">
@@ -978,7 +970,7 @@
       </c>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -995,10 +987,10 @@
         <f t="shared" si="0"/>
         <v>2105.4</v>
       </c>
-      <c r="F11" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G11" s="5">
+      <c r="F11" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G11" s="4">
         <v>44813</v>
       </c>
       <c r="H11" s="1">
@@ -1017,7 +1009,7 @@
       </c>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1034,10 +1026,10 @@
         <f t="shared" si="0"/>
         <v>2161.5</v>
       </c>
-      <c r="F12" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G12" s="5">
+      <c r="F12" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G12" s="4">
         <v>44814</v>
       </c>
       <c r="H12" s="1">
@@ -1056,7 +1048,7 @@
       </c>
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1073,10 +1065,10 @@
         <f t="shared" si="0"/>
         <v>2216.5</v>
       </c>
-      <c r="F13" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G13" s="5">
+      <c r="F13" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G13" s="4">
         <v>44815</v>
       </c>
       <c r="H13" s="1">
@@ -1095,7 +1087,7 @@
       </c>
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1112,10 +1104,10 @@
         <f t="shared" si="0"/>
         <v>2270.4</v>
       </c>
-      <c r="F14" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G14" s="5">
+      <c r="F14" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G14" s="4">
         <v>44816</v>
       </c>
       <c r="H14" s="1">
@@ -1134,7 +1126,7 @@
       </c>
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="A15" s="3">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1151,10 +1143,10 @@
         <f t="shared" si="0"/>
         <v>2323.2000000000003</v>
       </c>
-      <c r="F15" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G15" s="5">
+      <c r="F15" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G15" s="4">
         <v>44817</v>
       </c>
       <c r="H15" s="1">
@@ -1173,7 +1165,7 @@
       </c>
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+      <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1190,10 +1182,10 @@
         <f t="shared" si="0"/>
         <v>2374.9000000000005</v>
       </c>
-      <c r="F16" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G16" s="5">
+      <c r="F16" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G16" s="4">
         <v>44818</v>
       </c>
       <c r="H16" s="1">
@@ -1212,7 +1204,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+      <c r="A17" s="3">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1229,10 +1221,10 @@
         <f t="shared" si="0"/>
         <v>2425.5</v>
       </c>
-      <c r="F17" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G17" s="5">
+      <c r="F17" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G17" s="4">
         <v>44819</v>
       </c>
       <c r="H17" s="1">
@@ -1251,7 +1243,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+      <c r="A18" s="3">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1268,10 +1260,10 @@
         <f t="shared" si="0"/>
         <v>2475</v>
       </c>
-      <c r="F18" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G18" s="5">
+      <c r="F18" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G18" s="4">
         <v>44820</v>
       </c>
       <c r="H18" s="1">
@@ -1290,7 +1282,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+      <c r="A19" s="3">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1307,10 +1299,10 @@
         <f t="shared" si="0"/>
         <v>2523.4</v>
       </c>
-      <c r="F19" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G19" s="5">
+      <c r="F19" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G19" s="4">
         <v>44821</v>
       </c>
       <c r="H19" s="1">
@@ -1329,7 +1321,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+      <c r="A20" s="3">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1346,10 +1338,10 @@
         <f t="shared" si="0"/>
         <v>2570.7000000000003</v>
       </c>
-      <c r="F20" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G20" s="5">
+      <c r="F20" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G20" s="4">
         <v>44822</v>
       </c>
       <c r="H20" s="1">
@@ -1368,7 +1360,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+      <c r="A21" s="3">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1385,10 +1377,10 @@
         <f t="shared" si="0"/>
         <v>2616.9000000000005</v>
       </c>
-      <c r="F21" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G21" s="5">
+      <c r="F21" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G21" s="4">
         <v>44823</v>
       </c>
       <c r="H21" s="1">
@@ -1407,7 +1399,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+      <c r="A22" s="3">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1424,10 +1416,10 @@
         <f t="shared" si="0"/>
         <v>2662</v>
       </c>
-      <c r="F22" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G22" s="5">
+      <c r="F22" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G22" s="4">
         <v>44824</v>
       </c>
       <c r="H22" s="1">
@@ -1446,7 +1438,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
+      <c r="A23" s="3">
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1463,10 +1455,10 @@
         <f t="shared" si="0"/>
         <v>2706</v>
       </c>
-      <c r="F23" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G23" s="5">
+      <c r="F23" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G23" s="4">
         <v>44825</v>
       </c>
       <c r="H23" s="1">
@@ -1485,7 +1477,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
+      <c r="A24" s="3">
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1502,10 +1494,10 @@
         <f t="shared" si="0"/>
         <v>2748.9</v>
       </c>
-      <c r="F24" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G24" s="5">
+      <c r="F24" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G24" s="4">
         <v>44826</v>
       </c>
       <c r="H24" s="1">
@@ -1524,7 +1516,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
+      <c r="A25" s="3">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1541,10 +1533,10 @@
         <f t="shared" si="0"/>
         <v>2790.7000000000003</v>
       </c>
-      <c r="F25" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G25" s="5">
+      <c r="F25" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G25" s="4">
         <v>44827</v>
       </c>
       <c r="H25" s="1">
@@ -1563,7 +1555,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
+      <c r="A26" s="3">
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1580,10 +1572,10 @@
         <f t="shared" si="0"/>
         <v>2831.4000000000005</v>
       </c>
-      <c r="F26" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G26" s="5">
+      <c r="F26" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G26" s="4">
         <v>44828</v>
       </c>
       <c r="H26" s="1">
@@ -1602,7 +1594,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
+      <c r="A27" s="3">
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -1619,10 +1611,10 @@
         <f t="shared" si="0"/>
         <v>2871.0000000000005</v>
       </c>
-      <c r="F27" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G27" s="5">
+      <c r="F27" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G27" s="4">
         <v>44829</v>
       </c>
       <c r="H27" s="1">
@@ -1641,7 +1633,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
+      <c r="A28" s="3">
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1658,10 +1650,10 @@
         <f t="shared" si="0"/>
         <v>2909.5</v>
       </c>
-      <c r="F28" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G28" s="5">
+      <c r="F28" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G28" s="4">
         <v>44830</v>
       </c>
       <c r="H28" s="1">
@@ -1680,7 +1672,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
+      <c r="A29" s="3">
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1697,10 +1689,10 @@
         <f t="shared" si="0"/>
         <v>2946.9</v>
       </c>
-      <c r="F29" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G29" s="5">
+      <c r="F29" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G29" s="4">
         <v>44831</v>
       </c>
       <c r="H29" s="1">
@@ -1719,7 +1711,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
+      <c r="A30" s="3">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1736,10 +1728,10 @@
         <f t="shared" si="0"/>
         <v>2983.2000000000003</v>
       </c>
-      <c r="F30" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G30" s="5">
+      <c r="F30" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G30" s="4">
         <v>44832</v>
       </c>
       <c r="H30" s="1">
@@ -1758,7 +1750,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
+      <c r="A31" s="3">
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1775,10 +1767,10 @@
         <f t="shared" si="0"/>
         <v>3018.4000000000005</v>
       </c>
-      <c r="F31" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G31" s="5">
+      <c r="F31" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G31" s="4">
         <v>44833</v>
       </c>
       <c r="H31" s="1">
@@ -1797,7 +1789,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
+      <c r="A32" s="3">
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1814,10 +1806,10 @@
         <f t="shared" si="0"/>
         <v>3052.5000000000005</v>
       </c>
-      <c r="F32" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G32" s="5">
+      <c r="F32" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G32" s="4">
         <v>44834</v>
       </c>
       <c r="H32" s="1">
@@ -1836,7 +1828,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
+      <c r="A33" s="3">
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1853,10 +1845,10 @@
         <f t="shared" si="0"/>
         <v>3085.5</v>
       </c>
-      <c r="F33" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G33" s="5">
+      <c r="F33" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G33" s="4">
         <v>44835</v>
       </c>
       <c r="H33" s="1">
@@ -1875,7 +1867,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
+      <c r="A34" s="3">
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1892,10 +1884,10 @@
         <f t="shared" si="0"/>
         <v>3117.4</v>
       </c>
-      <c r="F34" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G34" s="5">
+      <c r="F34" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G34" s="4">
         <v>44836</v>
       </c>
       <c r="H34" s="1">
@@ -1914,7 +1906,7 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
+      <c r="A35" s="3">
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -1931,10 +1923,10 @@
         <f t="shared" si="0"/>
         <v>1574.1000000000001</v>
       </c>
-      <c r="F35" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G35" s="5">
+      <c r="F35" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G35" s="4">
         <v>44837</v>
       </c>
       <c r="H35" s="1">
@@ -1953,7 +1945,7 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
+      <c r="A36" s="3">
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1970,10 +1962,10 @@
         <f t="shared" si="0"/>
         <v>1588.95</v>
       </c>
-      <c r="F36" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G36" s="5">
+      <c r="F36" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G36" s="4">
         <v>44838</v>
       </c>
       <c r="H36" s="1">
@@ -1992,7 +1984,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
+      <c r="A37" s="3">
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -2009,10 +2001,10 @@
         <f t="shared" si="0"/>
         <v>1603.2500000000002</v>
       </c>
-      <c r="F37" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G37" s="5">
+      <c r="F37" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G37" s="4">
         <v>44839</v>
       </c>
       <c r="H37" s="1">
@@ -2031,7 +2023,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="2">
+      <c r="A38" s="3">
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -2048,10 +2040,10 @@
         <f t="shared" si="0"/>
         <v>1617.0000000000002</v>
       </c>
-      <c r="F38" s="5">
-        <v>44813</v>
-      </c>
-      <c r="G38" s="5">
+      <c r="F38" s="4">
+        <v>44813</v>
+      </c>
+      <c r="G38" s="4">
         <v>44840</v>
       </c>
       <c r="H38" s="1">
@@ -2109,30 +2101,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>